<commit_message>
Burndown Chart Sprint 2
Burndown chart and graph for sprint 2
</commit_message>
<xml_diff>
--- a/Burndown Chart Sprint 1.xlsx
+++ b/Burndown Chart Sprint 1.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkala\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Denis\Documents\GitHub\SaveTheWorld\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E83B09-BDD9-4B76-BFF1-94741CC4D578}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F9D5F6A-F267-42B2-8765-7463474C2AB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{CE30A7DE-2A8D-409E-8E48-71CE7DD8FD12}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8863" activeTab="1" xr2:uid="{CE30A7DE-2A8D-409E-8E48-71CE7DD8FD12}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t xml:space="preserve">Day 1 </t>
   </si>
@@ -124,7 +125,7 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -142,7 +143,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="cs-CZ"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -624,6 +625,432 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="hr-HR"/>
+              <a:t>Sprint 2</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual streamline</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$5:$F$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Day 1 </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day 2 </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day 3 </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Day 4 </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$6:$F$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-32FB-4EEA-8921-2F318B39B016}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Desired streamline</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$5:$F$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Day 1 </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day 2 </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day 3 </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Day 4 </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$7:$F$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-32FB-4EEA-8921-2F318B39B016}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1609892447"/>
+        <c:axId val="1604067375"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1609892447"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1604067375"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1604067375"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1609892447"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -664,7 +1091,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1221,8 +2204,49 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>601436</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>40821</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>601436</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>8164</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A9382B5-95FC-45D8-AFD9-6002261D49D2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1520,19 +2544,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F43EEC3-5B81-4898-999A-FA2117FE2DAF}">
   <dimension ref="A2:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.15234375" customWidth="1"/>
+    <col min="2" max="2" width="18.69140625" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="12" max="12" width="22.42578125" customWidth="1"/>
+    <col min="12" max="12" width="22.3828125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -1561,7 +2585,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1593,7 +2617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1625,61 +2649,61 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9" s="3"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" s="3"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11" s="3"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" s="3"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13" s="3"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A14" s="3"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15" s="3"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A16" s="3"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17" s="3"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" s="3"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="6:6" x14ac:dyDescent="0.4">
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="6:6" x14ac:dyDescent="0.4">
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="6:6" x14ac:dyDescent="0.4">
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="6:6" x14ac:dyDescent="0.4">
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="6:6" x14ac:dyDescent="0.4">
       <c r="F37" s="2"/>
     </row>
   </sheetData>
@@ -1687,4 +2711,71 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81EC2EFD-9A51-42D6-B811-289FB576E00E}">
+  <dimension ref="B5:F7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="2" max="2" width="17.3046875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>140</v>
+      </c>
+      <c r="D6">
+        <v>100</v>
+      </c>
+      <c r="E6">
+        <v>45</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>140</v>
+      </c>
+      <c r="D7">
+        <v>95</v>
+      </c>
+      <c r="E7">
+        <v>50</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>